<commit_message>
suppr draft et decomment dans CapabilityStatement 7197940fbc3eddd61149790a71852ae0788ae85f
</commit_message>
<xml_diff>
--- a/suppr-draft-sp-type-orga/ig/StructureDefinition-ror-healthcareservice.xlsx
+++ b/suppr-draft-sp-type-orga/ig/StructureDefinition-ror-healthcareservice.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-02-13T16:52:13+00:00</t>
+    <t>2025-02-17T10:19:56+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -12697,10 +12697,10 @@
         <v>85</v>
       </c>
       <c r="G92" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="H92" t="s" s="2">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="I92" t="s" s="2">
         <v>75</v>
@@ -12709,13 +12709,13 @@
         <v>75</v>
       </c>
       <c r="K92" t="s" s="2">
-        <v>110</v>
+        <v>446</v>
       </c>
       <c r="L92" t="s" s="2">
-        <v>198</v>
+        <v>447</v>
       </c>
       <c r="M92" t="s" s="2">
-        <v>199</v>
+        <v>448</v>
       </c>
       <c r="N92" s="2"/>
       <c r="O92" s="2"/>
@@ -13799,10 +13799,10 @@
         <v>85</v>
       </c>
       <c r="G102" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="H102" t="s" s="2">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="I102" t="s" s="2">
         <v>75</v>
@@ -13811,13 +13811,13 @@
         <v>75</v>
       </c>
       <c r="K102" t="s" s="2">
-        <v>110</v>
+        <v>446</v>
       </c>
       <c r="L102" t="s" s="2">
-        <v>198</v>
+        <v>447</v>
       </c>
       <c r="M102" t="s" s="2">
-        <v>199</v>
+        <v>448</v>
       </c>
       <c r="N102" s="2"/>
       <c r="O102" s="2"/>

</xml_diff>